<commit_message>
Working menu and settings
Menu and settings window are working correct, settings save to computer and load once game is loaded.
</commit_message>
<xml_diff>
--- a/Assets/Project structure/Small scripts.xlsx
+++ b/Assets/Project structure/Small scripts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>GetTextByLanguage</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Loads users settings when game is opened</t>
+  </si>
+  <si>
+    <t>SettingsScene</t>
   </si>
 </sst>
 </file>
@@ -385,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C7"/>
+  <dimension ref="B2:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,6 +442,11 @@
         <v>9</v>
       </c>
     </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Working menu and settings (upd 1)
</commit_message>
<xml_diff>
--- a/Assets/Project structure/Small scripts.xlsx
+++ b/Assets/Project structure/Small scripts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>GetTextByLanguage</t>
   </si>
@@ -47,13 +47,28 @@
   </si>
   <si>
     <t>SettingsScene</t>
+  </si>
+  <si>
+    <t>Deactivates object on start</t>
+  </si>
+  <si>
+    <t>DeactivateOnStart</t>
+  </si>
+  <si>
+    <t>Global initialization</t>
+  </si>
+  <si>
+    <t>Script, that attaches to button that load scene on click</t>
+  </si>
+  <si>
+    <t>Script that is on settings scene, saving settings that user sets</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,16 +76,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -78,12 +115,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
@@ -388,63 +442,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C8"/>
+  <dimension ref="B2:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="100.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="124" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working player (upd 1) and 3D models
Player scripts were updated and divided into 2 classes (PersonController and MouseRotation). Some 3D models were imported.
</commit_message>
<xml_diff>
--- a/Assets/Project structure/Small scripts.xlsx
+++ b/Assets/Project structure/Small scripts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>GetTextByLanguage</t>
   </si>
@@ -62,13 +62,25 @@
   </si>
   <si>
     <t>Script that is on settings scene, saving settings that user sets</t>
+  </si>
+  <si>
+    <t>PersonController</t>
+  </si>
+  <si>
+    <t>Controls players movement</t>
+  </si>
+  <si>
+    <t>MouseRotation</t>
+  </si>
+  <si>
+    <t>Rotates objects according to mouse position</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +102,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -134,13 +154,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -158,7 +179,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -196,7 +217,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -268,7 +289,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -442,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C9"/>
+  <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -518,6 +539,22 @@
         <v>11</v>
       </c>
     </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>